<commit_message>
update with turnkey notes
</commit_message>
<xml_diff>
--- a/hardware/permamote/rev_a/permamote_bom.xlsx
+++ b/hardware/permamote/rev_a/permamote_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="271">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">OC_NEWARK</t>
   </si>
   <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.1uF</t>
   </si>
   <si>
@@ -526,6 +529,9 @@
     <t xml:space="preserve">BAT-HLD-001-THM-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">Do Not Populate</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAT_PACKCR123A</t>
   </si>
   <si>
@@ -646,6 +652,9 @@
     <t xml:space="preserve">ISL29125IROZ-T7A</t>
   </si>
   <si>
+    <t xml:space="preserve">Will Provide (Part is out of stock everywhere)</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIS2DW12</t>
   </si>
   <si>
@@ -764,6 +773,9 @@
   </si>
   <si>
     <t xml:space="preserve">NORIDIC SEMICONDUCTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will Provide (Part is not yet in production)</t>
   </si>
   <si>
     <t xml:space="preserve">PMDXB950UPEL</t>
@@ -835,6 +847,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -916,27 +929,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="36:37"/>
+      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="33.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="134.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="108.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="108.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,31 +996,34 @@
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,25 +1031,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,25 +1057,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,25 +1083,25 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,25 +1109,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,25 +1135,25 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,25 +1161,25 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,25 +1187,25 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,25 +1213,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,25 +1239,25 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,25 +1265,25 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1274,25 +1291,25 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,28 +1317,28 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,22 +1346,22 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>74437324220</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>74437324220</v>
@@ -1355,25 +1372,25 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,25 +1398,25 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,28 +1424,28 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,28 +1453,28 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,25 +1482,25 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1491,25 +1508,25 @@
         <v>3</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,22 +1537,22 @@
         <v>470</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,25 +1560,25 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,25 +1586,25 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,25 +1612,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,25 +1638,25 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,25 +1664,25 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,25 +1690,25 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,25 +1716,25 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,28 +1742,28 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D30" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="K30" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1754,28 +1771,28 @@
         <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,28 +1800,28 @@
         <v>1</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E32" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="K32" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="K32" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,25 +1829,28 @@
         <v>2</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E33" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="K33" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="K33" s="0" t="s">
-        <v>164</v>
+      <c r="O33" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,27 +1858,30 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F34" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="K34" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="G34" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="K34" s="0" t="s">
+      <c r="O34" s="0" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1867,28 +1890,28 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,19 +1919,22 @@
         <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="O36" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,22 +1942,25 @@
         <v>5</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
+      </c>
+      <c r="O37" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1939,28 +1968,28 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E38" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="K38" s="0" t="s">
         <v>187</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="K38" s="0" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,25 +1997,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,28 +2023,28 @@
         <v>1</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E40" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="K40" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="K40" s="0" t="s">
-        <v>196</v>
       </c>
       <c r="M40" s="0" t="n">
         <v>1146033</v>
       </c>
       <c r="N40" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,28 +2052,31 @@
         <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
+      </c>
+      <c r="O41" s="0" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,28 +2084,28 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2081,28 +2113,28 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,28 +2142,28 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2139,25 +2171,25 @@
         <v>1</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="K45" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,28 +2197,28 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,28 +2226,31 @@
         <v>1</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F47" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="K47" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="G47" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="K47" s="0" t="s">
-        <v>242</v>
+      <c r="O47" s="0" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,28 +2258,28 @@
         <v>9</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2252,28 +2287,28 @@
         <v>1</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="G49" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="K49" s="0" t="s">
         <v>259</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="K49" s="0" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,28 +2316,28 @@
         <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="G50" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="K50" s="0" t="s">
         <v>265</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="K50" s="0" t="s">
-        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change attributes to include MPN, fix up BOM
</commit_message>
<xml_diff>
--- a/hardware/permamote/rev_a/permamote_bom.xlsx
+++ b/hardware/permamote/rev_a/permamote_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="272">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -127,10 +127,10 @@
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">541-100MAHCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRCW0603100MJPEAHR</t>
+    <t xml:space="preserve">HMC0402JT100MCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMC0402JT100M</t>
   </si>
   <si>
     <t xml:space="preserve">100pF</t>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve">RC0402JR-0710KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do Not Populate R6 &amp; R7</t>
   </si>
   <si>
     <t xml:space="preserve">10nF</t>
@@ -932,7 +935,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
+      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -941,7 +944,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="33.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="134.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="108.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="108.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.21"/>
@@ -949,7 +952,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1155,13 +1158,16 @@
       <c r="K7" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="O7" s="0" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>16</v>
@@ -1170,16 +1176,16 @@
         <v>17</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,25 +1193,25 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,25 +1219,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1239,7 +1245,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>16</v>
@@ -1248,16 +1254,16 @@
         <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,25 +1271,25 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,7 +1297,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>16</v>
@@ -1300,16 +1306,16 @@
         <v>17</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1317,28 +1323,28 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,22 +1352,22 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>74437324220</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>74437324220</v>
@@ -1372,25 +1378,25 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>31</v>
@@ -1407,16 +1413,16 @@
         <v>32</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1424,28 +1430,28 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="K18" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,28 +1459,28 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,25 +1488,25 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,7 +1514,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>16</v>
@@ -1517,16 +1523,16 @@
         <v>17</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>19</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,16 +1549,16 @@
         <v>32</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1560,7 +1566,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>16</v>
@@ -1569,16 +1575,16 @@
         <v>17</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>19</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>16</v>
@@ -1595,16 +1601,16 @@
         <v>17</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>19</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,7 +1618,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>31</v>
@@ -1621,16 +1627,16 @@
         <v>32</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>31</v>
@@ -1647,16 +1653,16 @@
         <v>32</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>31</v>
@@ -1673,16 +1679,16 @@
         <v>32</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,25 +1696,25 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>31</v>
@@ -1725,16 +1731,16 @@
         <v>32</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,28 +1748,28 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D30" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,28 +1777,28 @@
         <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1800,28 +1806,28 @@
         <v>1</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E32" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="K32" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="K32" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,28 +1835,28 @@
         <v>2</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E33" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="K33" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="K33" s="0" t="s">
-        <v>165</v>
-      </c>
       <c r="O33" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,31 +1864,31 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="O34" s="0" t="s">
         <v>170</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="O34" s="0" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,28 +1896,28 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1919,7 +1925,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>16</v>
@@ -1928,13 +1934,13 @@
         <v>17</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>19</v>
       </c>
       <c r="O36" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,7 +1948,7 @@
         <v>5</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>31</v>
@@ -1951,16 +1957,16 @@
         <v>32</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O37" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,28 +1974,28 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D38" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="K38" s="0" t="s">
         <v>188</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="K38" s="0" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,25 +2003,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,28 +2029,28 @@
         <v>1</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D40" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="K40" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="K40" s="0" t="s">
-        <v>198</v>
       </c>
       <c r="M40" s="0" t="n">
         <v>1146033</v>
       </c>
       <c r="N40" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,31 +2058,31 @@
         <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O41" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2084,28 +2090,28 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,28 +2119,28 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,28 +2148,28 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,25 +2177,25 @@
         <v>1</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="K45" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,28 +2203,28 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,31 +2232,31 @@
         <v>1</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D47" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="K47" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E47" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="K47" s="0" t="s">
-        <v>245</v>
-      </c>
       <c r="O47" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2258,28 +2264,28 @@
         <v>9</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,28 +2293,28 @@
         <v>1</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D49" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="K49" s="0" t="s">
         <v>260</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="K49" s="0" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2316,28 +2322,28 @@
         <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D50" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="K50" s="0" t="s">
         <v>266</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="K50" s="0" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix NRF52840 via drill size
Update BOM
</commit_message>
<xml_diff>
--- a/hardware/permamote/rev_a/permamote_bom.xlsx
+++ b/hardware/permamote/rev_a/permamote_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="282">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">490-6328-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM155R71C104KA88J</t>
+    <t xml:space="preserve">GRM155R71C104KA88J </t>
   </si>
   <si>
     <t xml:space="preserve">0.5pF</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">490-6264-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM1555C1HR50WA01D</t>
+    <t xml:space="preserve">GRM1555C1HR50WA01D </t>
   </si>
   <si>
     <t xml:space="preserve">0.8pF</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">490-6269-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM1555C1HR80BA01D</t>
+    <t xml:space="preserve">GRM1555C1HR80BA01D </t>
   </si>
   <si>
     <t xml:space="preserve">100M</t>
@@ -127,10 +127,10 @@
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">HMC0402JT100MCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HMC0402JT100M</t>
+    <t xml:space="preserve">541-100MAHCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMC0402JT100M </t>
   </si>
   <si>
     <t xml:space="preserve">100pF</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">490-5922-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM1555C1H101JA01D</t>
+    <t xml:space="preserve">GRM1555C1H101JA01D </t>
   </si>
   <si>
     <t xml:space="preserve">10k</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">RC0402JR-0710KL</t>
   </si>
   <si>
-    <t xml:space="preserve">Do Not Populate R6 &amp; R7</t>
+    <t xml:space="preserve">Do not populate R6 &amp; R7</t>
   </si>
   <si>
     <t xml:space="preserve">10nF</t>
@@ -169,7 +169,7 @@
     <t xml:space="preserve">490-4516-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM155R71H103KA88D</t>
+    <t xml:space="preserve">GRM155R71H103KA88D </t>
   </si>
   <si>
     <t xml:space="preserve">10uF</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">490-3896-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM188R60J106ME47D</t>
+    <t xml:space="preserve">GRM188R60J106ME47D </t>
   </si>
   <si>
     <t xml:space="preserve">10uH</t>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">490-4025-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">LQM18FN100M00D</t>
+    <t xml:space="preserve">LQM18FN100M00D </t>
   </si>
   <si>
     <t xml:space="preserve">12pF</t>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">490-6197-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM1555C1H120GA01D</t>
+    <t xml:space="preserve">GRM1555C1H120GA01D </t>
   </si>
   <si>
     <t xml:space="preserve">15nH</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">587-1521-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">HK100515NJ-T</t>
+    <t xml:space="preserve">HK100515NJ-T </t>
   </si>
   <si>
     <t xml:space="preserve">1uF</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">490-7195-1-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">GRM155R70G105KA12D</t>
+    <t xml:space="preserve">GRM155R70G105KA12D </t>
   </si>
   <si>
     <t xml:space="preserve">1uH</t>
@@ -289,7 +289,7 @@
     <t xml:space="preserve">535-10426-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">AISC-0402-3N3J-T</t>
+    <t xml:space="preserve">AISC-0402-3N3J-T </t>
   </si>
   <si>
     <t xml:space="preserve">3.9M</t>
@@ -364,7 +364,7 @@
     <t xml:space="preserve">HMC0603JT33M0CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">HMC0603JT33M0</t>
+    <t xml:space="preserve">HMC0603JT33M0 </t>
   </si>
   <si>
     <t xml:space="preserve">4.7uF</t>
@@ -376,7 +376,7 @@
     <t xml:space="preserve">445-5947-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">C1005X5R0J475K050BC</t>
+    <t xml:space="preserve">C1005X5R0J475K050BC </t>
   </si>
   <si>
     <t xml:space="preserve">R1, R2, R3</t>
@@ -385,7 +385,7 @@
     <t xml:space="preserve">311-470JRCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">RC0402JR-07470RL</t>
+    <t xml:space="preserve">RC0402JR-07470RL </t>
   </si>
   <si>
     <t xml:space="preserve">47nF</t>
@@ -397,7 +397,7 @@
     <t xml:space="preserve">445-1264-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">C1005X7R1C473K050BC</t>
+    <t xml:space="preserve">C1005X7R1C473K050BC </t>
   </si>
   <si>
     <t xml:space="preserve">47pF</t>
@@ -409,7 +409,7 @@
     <t xml:space="preserve">490-5942-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM1555C1H470JA01D</t>
+    <t xml:space="preserve">GRM1555C1H470JA01D </t>
   </si>
   <si>
     <t xml:space="preserve">6.04k</t>
@@ -457,7 +457,7 @@
     <t xml:space="preserve">311-80.6KHRCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">RC0603FR-0780K6L</t>
+    <t xml:space="preserve">RC0603FR-0780K6L </t>
   </si>
   <si>
     <t xml:space="preserve">9.1M</t>
@@ -520,19 +520,25 @@
     <t xml:space="preserve">YAGEO</t>
   </si>
   <si>
+    <t xml:space="preserve">BAT-HLD-002-THM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT2, BT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RETAINER BATT CR2016 PC PINS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAT-HLD-001-THM-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">712-BAT-HLD-001-THM</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAT-HLD-001-THM</t>
   </si>
   <si>
-    <t xml:space="preserve">BT2, BT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAINER BATT CR2032 PC PINS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAT-HLD-001-THM-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do Not Populate</t>
+    <t xml:space="preserve">Do not populate</t>
   </si>
   <si>
     <t xml:space="preserve">BAT_PACKCR123A</t>
@@ -616,7 +622,7 @@
     <t xml:space="preserve">P11084SCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">EVQ-P2K02Q</t>
+    <t xml:space="preserve">EVQ-P2K02Q </t>
   </si>
   <si>
     <t xml:space="preserve">FT232RQ</t>
@@ -655,7 +661,7 @@
     <t xml:space="preserve">ISL29125IROZ-T7A</t>
   </si>
   <si>
-    <t xml:space="preserve">Will Provide (Part is out of stock everywhere)</t>
+    <t xml:space="preserve">Will Consign (Part is out of stock everywhere)</t>
   </si>
   <si>
     <t xml:space="preserve">LIS2DW12</t>
@@ -679,6 +685,12 @@
     <t xml:space="preserve">LIS2DW12TR</t>
   </si>
   <si>
+    <t xml:space="preserve">LTOHTC1020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT1</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAX17222</t>
   </si>
   <si>
@@ -721,10 +733,7 @@
     <t xml:space="preserve">MAX44009EDT+T</t>
   </si>
   <si>
-    <t xml:space="preserve">MICRO_USB_B_HIROSE_ZX62R-B-5P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB_MICRO_B-HIROSE-ZX62R-B-5P</t>
+    <t xml:space="preserve">MICRO_USB_B_HIROSE_ZX62R-B-5P(30)</t>
   </si>
   <si>
     <t xml:space="preserve">J5</t>
@@ -736,9 +745,15 @@
     <t xml:space="preserve">H125274CT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">798-ZX62R-B-5P30</t>
+  </si>
+  <si>
     <t xml:space="preserve">ZX62R-B-5P(30)</t>
   </si>
   <si>
+    <t xml:space="preserve">84Y6712</t>
+  </si>
+  <si>
     <t xml:space="preserve">MS5637-02BA03</t>
   </si>
   <si>
@@ -778,7 +793,7 @@
     <t xml:space="preserve">NORIDIC SEMICONDUCTOR</t>
   </si>
   <si>
-    <t xml:space="preserve">Will Provide (Part is not yet in production)</t>
+    <t xml:space="preserve">Will Consign (Part is not yet in production)</t>
   </si>
   <si>
     <t xml:space="preserve">PMDXB950UPEL</t>
@@ -820,6 +835,9 @@
     <t xml:space="preserve">634-SI7021-A20-GM1</t>
   </si>
   <si>
+    <t xml:space="preserve">SI7021-A20-GM1 </t>
+  </si>
+  <si>
     <t xml:space="preserve">SML-LX0404SIUPGUSB</t>
   </si>
   <si>
@@ -836,6 +854,18 @@
   </si>
   <si>
     <t xml:space="preserve">Lumex Opto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOLARCELLHOLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOLAR_HOLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic solar cell</t>
   </si>
 </sst>
 </file>
@@ -850,7 +880,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -932,27 +961,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O50"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
+      <selection pane="topLeft" activeCell="O49" activeCellId="0" sqref="O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="33.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="36.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="134.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="108.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="108.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.51"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1852,11 +1880,14 @@
       <c r="G33" s="0" t="s">
         <v>169</v>
       </c>
+      <c r="J33" s="0" t="s">
+        <v>170</v>
+      </c>
       <c r="K33" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,31 +1895,31 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D34" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="O34" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="O34" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,28 +1927,28 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,7 +1956,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>16</v>
@@ -1934,13 +1965,13 @@
         <v>17</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>19</v>
       </c>
       <c r="O36" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1948,7 +1979,7 @@
         <v>5</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>31</v>
@@ -1957,16 +1988,16 @@
         <v>32</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>34</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O37" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,28 +2005,28 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E38" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="K38" s="0" t="s">
         <v>190</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="K38" s="0" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2003,25 +2034,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2029,28 +2060,28 @@
         <v>1</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E40" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="K40" s="0" t="s">
         <v>201</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="K40" s="0" t="s">
-        <v>199</v>
       </c>
       <c r="M40" s="0" t="n">
         <v>1146033</v>
       </c>
       <c r="N40" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,31 +2089,31 @@
         <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="O41" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,28 +2121,28 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,28 +2150,19 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>1020</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="F43" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="G43" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="K43" s="0" t="s">
-        <v>225</v>
+      <c r="O43" s="0" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2148,28 +2170,28 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="F44" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="D44" s="0" t="s">
+      <c r="G44" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="H44" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="K44" s="0" t="s">
         <v>229</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="K44" s="0" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2177,25 +2199,28 @@
         <v>1</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="D45" s="0" t="s">
+      <c r="G45" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="H45" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="K45" s="0" t="s">
         <v>236</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="K45" s="0" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2203,28 +2228,31 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="F46" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="D46" s="0" t="s">
+      <c r="G46" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="J46" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="K46" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="L46" s="0" t="s">
         <v>243</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="K46" s="0" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,89 +2260,89 @@
         <v>1</v>
       </c>
       <c r="B47" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="D47" s="0" t="s">
+      <c r="F47" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="G47" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="H47" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="G47" s="0" t="s">
+      <c r="K47" s="0" t="s">
         <v>250</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="K47" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="O47" s="0" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B48" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="E48" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="D48" s="0" t="s">
+      <c r="F48" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="G48" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="H48" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="G48" s="0" t="s">
+      <c r="K48" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="O48" s="0" t="s">
         <v>257</v>
-      </c>
-      <c r="H48" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="K48" s="0" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B49" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="E49" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="C49" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="D49" s="0" t="s">
+      <c r="F49" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="G49" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="F49" s="0" t="s">
+      <c r="H49" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="G49" s="0" t="s">
+      <c r="K49" s="0" t="s">
         <v>264</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="K49" s="0" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,28 +2350,80 @@
         <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="C50" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="D50" s="0" t="s">
+      <c r="E50" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="F50" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="G50" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="G50" s="0" t="s">
+      <c r="J50" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="H50" s="0" t="s">
+      <c r="K50" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="K50" s="0" t="s">
-        <v>266</v>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="K51" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="O52" s="0" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>